<commit_message>
updated readme files on patterns
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32121D8-389D-482D-8C31-2440A8487C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A0FCF4-57E1-4C06-975E-59C4018FACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="96">
   <si>
     <t>Week</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -504,6 +507,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -524,62 +552,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -597,16 +580,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -944,7 +917,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,28 +931,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -992,7 +965,7 @@
       <c r="G2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="10" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1013,9 +986,9 @@
         <v>6</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="25" t="s">
-        <v>94</v>
+      <c r="G3" s="7"/>
+      <c r="H3" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1035,9 +1008,9 @@
         <v>7</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="25" t="s">
-        <v>94</v>
+      <c r="G4" s="7"/>
+      <c r="H4" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1057,8 +1030,8 @@
         <v>10</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1079,8 +1052,8 @@
         <v>11</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="25" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1101,8 +1074,8 @@
         <v>14</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="25" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1123,8 +1096,8 @@
         <v>15</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1145,8 +1118,8 @@
         <v>18</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="25" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1167,44 +1140,44 @@
         <v>19</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="25" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="16">
         <v>2</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="16">
         <v>3</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="25" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="25" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1225,8 +1198,8 @@
         <v>23</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="25" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1247,8 +1220,8 @@
         <v>24</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="25" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1269,8 +1242,8 @@
         <v>27</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="25" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1291,10 +1264,10 @@
         <v>30</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1315,10 +1288,10 @@
         <v>32</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1339,10 +1312,10 @@
         <v>34</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1365,10 +1338,10 @@
       <c r="F19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1391,10 +1364,10 @@
       <c r="F20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1411,10 +1384,10 @@
       <c r="F21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1431,10 +1404,10 @@
       <c r="F22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1451,10 +1424,10 @@
       <c r="F23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1471,10 +1444,10 @@
       <c r="F24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1497,10 +1470,10 @@
       <c r="F25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1521,8 +1494,8 @@
         <v>53</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="25" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1543,8 +1516,8 @@
         <v>55</v>
       </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="25" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1565,8 +1538,8 @@
         <v>56</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="25" t="s">
+      <c r="G28" s="7"/>
+      <c r="H28" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1587,8 +1560,8 @@
         <v>57</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="25" t="s">
+      <c r="G29" s="7"/>
+      <c r="H29" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1609,48 +1582,48 @@
         <v>59</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="25" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
+      <c r="A31" s="16">
         <v>5</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="16">
         <v>1</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="25" t="s">
+      <c r="H31" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="23" t="s">
+      <c r="A32" s="17"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H32" s="25" t="s">
+      <c r="H32" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1673,10 +1646,10 @@
       <c r="F33" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1699,10 +1672,10 @@
       <c r="F34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1725,10 +1698,10 @@
       <c r="F35" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1749,8 +1722,8 @@
         <v>67</v>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="25" t="s">
+      <c r="G36" s="7"/>
+      <c r="H36" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1771,8 +1744,8 @@
         <v>67</v>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="25" t="s">
+      <c r="G37" s="7"/>
+      <c r="H37" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1795,10 +1768,10 @@
       <c r="F38" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H38" s="25" t="s">
+      <c r="H38" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1821,10 +1794,10 @@
       <c r="F39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1847,10 +1820,10 @@
       <c r="F40" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1873,10 +1846,10 @@
       <c r="F41" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="25" t="s">
+      <c r="H41" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1899,10 +1872,10 @@
       <c r="F42" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1923,8 +1896,8 @@
         <v>67</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="25" t="s">
+      <c r="G43" s="7"/>
+      <c r="H43" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1945,8 +1918,8 @@
         <v>67</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="25" t="s">
+      <c r="G44" s="7"/>
+      <c r="H44" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1967,8 +1940,8 @@
         <v>67</v>
       </c>
       <c r="F45" s="4"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="25" t="s">
+      <c r="G45" s="7"/>
+      <c r="H45" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1989,8 +1962,8 @@
         <v>67</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="25" t="s">
+      <c r="G46" s="7"/>
+      <c r="H46" s="11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2011,13 +1984,21 @@
         <v>67</v>
       </c>
       <c r="F47" s="4"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="25" t="s">
+      <c r="G47" s="7"/>
+      <c r="H47" s="11" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2027,23 +2008,13 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H47">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -2056,15 +2027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2324,6 +2286,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2336,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2359,6 +2322,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated readme for search functions
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A0FCF4-57E1-4C06-975E-59C4018FACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD81047-F90E-46CB-8298-DEC1E16677B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -520,26 +520,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,6 +537,26 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,7 +917,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,28 +931,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="7"/>
       <c r="H5" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1146,37 +1146,37 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="18">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="18">
         <v>3</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="25"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="11" t="s">
         <v>94</v>
       </c>
@@ -1588,22 +1588,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="16">
+      <c r="A31" s="18">
         <v>5</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="18">
         <v>1</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="20" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="8" t="s">
@@ -1614,12 +1614,12 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="19"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="9" t="s">
         <v>64</v>
       </c>
@@ -1991,11 +1991,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
@@ -2008,6 +2003,11 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,6 +2027,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2286,15 +2295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,6 +2307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2322,14 +2330,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
completed Financial Forecasting using recursion
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD81047-F90E-46CB-8298-DEC1E16677B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C94120-3AFC-47EE-B2BD-42D10B5555CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -520,24 +520,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -557,6 +539,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,7 +917,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,28 +931,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="7"/>
       <c r="H6" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1146,37 +1146,37 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="A11" s="12">
         <v>2</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="12">
         <v>3</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="11" t="s">
         <v>94</v>
       </c>
@@ -1588,22 +1588,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="18">
+      <c r="A31" s="12">
         <v>5</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="12">
         <v>1</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="14" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="8" t="s">
@@ -1614,12 +1614,12 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="19"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="21"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="15"/>
       <c r="G32" s="9" t="s">
         <v>64</v>
       </c>
@@ -1991,6 +1991,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
@@ -2007,7 +2008,6 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,15 +2027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2295,6 +2286,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2330,6 +2322,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add PL/SQL control structures exercises
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C94120-3AFC-47EE-B2BD-42D10B5555CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4BE821-D713-4FC8-8085-041A1FF6F9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -916,8 +916,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,7 +1076,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="7"/>
       <c r="H7" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1098,7 +1098,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="7"/>
       <c r="H8" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1991,10 +1991,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2004,10 +2003,11 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="G11:G12"/>
     <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
adding solutions for JUnit Test Exercises
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4BE821-D713-4FC8-8085-041A1FF6F9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8634C7B2-E1C7-4255-8EA2-91561BF29D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -520,26 +520,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,6 +536,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -917,7 +917,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,28 +931,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1120,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
       <c r="H9" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1142,43 +1142,43 @@
       <c r="F10" s="4"/>
       <c r="G10" s="7"/>
       <c r="H10" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="22">
         <v>2</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="22">
         <v>3</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1588,22 +1588,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="12">
+      <c r="A31" s="22">
         <v>5</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="22">
         <v>1</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="24" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="8" t="s">
@@ -1614,12 +1614,12 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="15"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="9" t="s">
         <v>64</v>
       </c>
@@ -1991,23 +1991,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,6 +2027,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2286,15 +2295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,6 +2307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2322,14 +2330,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adding solutions for mockito exercises
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8634C7B2-E1C7-4255-8EA2-91561BF29D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2231E504-A11E-4F81-90BC-2D29030C00D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -520,6 +520,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,14 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,7 +917,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11:G12"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,28 +931,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1146,37 +1146,37 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="12">
         <v>2</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="12">
         <v>3</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="11" t="s">
         <v>95</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="7"/>
       <c r="H13" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1222,7 +1222,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="7"/>
       <c r="H14" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1588,22 +1588,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="22">
+      <c r="A31" s="12">
         <v>5</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="12">
         <v>1</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="14" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="8" t="s">
@@ -1614,12 +1614,12 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="25"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="15"/>
       <c r="G32" s="9" t="s">
         <v>64</v>
       </c>
@@ -1991,12 +1991,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -2008,6 +2002,12 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,15 +2027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2295,6 +2286,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2330,6 +2322,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adding solutions for SLF4J excercise - completed week 2 mandatory excercises
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2231E504-A11E-4F81-90BC-2D29030C00D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F1F546-DE9E-4FD8-8917-4F2F6BA16085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -917,7 +917,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1244,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="7"/>
       <c r="H15" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1991,6 +1991,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -2002,12 +2008,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,6 +2027,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2286,15 +2295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,6 +2307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2322,14 +2330,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adding solutions for spring core and maven exercises - week 3
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F1F546-DE9E-4FD8-8917-4F2F6BA16085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB3F7F6-C43B-4909-BFE7-6A8909DDBD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -916,8 +916,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,7 +1268,7 @@
         <v>31</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1292,7 +1292,7 @@
         <v>33</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1316,7 +1316,7 @@
         <v>35</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1991,12 +1991,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -2008,6 +2002,12 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,15 +2027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2295,6 +2286,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2330,6 +2322,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added week 3 mandatory handson - spring jpa ,hibernate
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB3F7F6-C43B-4909-BFE7-6A8909DDBD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7CD26B-1B61-44CD-BC86-319F4FFA656A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -916,8 +916,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,7 +1342,7 @@
         <v>39</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1368,7 +1368,7 @@
         <v>41</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1991,6 +1991,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -2002,12 +2008,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,6 +2027,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2286,15 +2295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,6 +2307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2322,14 +2330,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adding week 4 JWT handson solutions
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7CD26B-1B61-44CD-BC86-319F4FFA656A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E06D83-958E-4D2E-9648-FEB084A0A637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -916,8 +916,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,7 +1474,7 @@
         <v>52</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1496,7 +1496,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="7"/>
       <c r="H26" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1518,7 +1518,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="7"/>
       <c r="H27" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1540,7 +1540,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="7"/>
       <c r="H28" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1562,7 +1562,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="7"/>
       <c r="H29" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1584,7 +1584,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="7"/>
       <c r="H30" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1991,12 +1991,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -2008,6 +2002,12 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,15 +2027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2295,6 +2286,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2330,6 +2322,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adding week 6 react HOL exercises and images
</commit_message>
<xml_diff>
--- a/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
+++ b/DN 4.0 - Java FSE Mandatory hands-on detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CTS_DN_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E06D83-958E-4D2E-9648-FEB084A0A637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B034A0D9-F85B-46D6-9842-4B7AF8D9FD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E078EC40-2268-4F4F-B14B-9403122955B8}"/>
   </bookViews>
@@ -916,8 +916,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1610,7 +1610,7 @@
         <v>63</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1624,7 +1624,7 @@
         <v>64</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1650,7 +1650,7 @@
         <v>67</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1676,7 +1676,7 @@
         <v>67</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1702,7 +1702,7 @@
         <v>67</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1724,7 +1724,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="7"/>
       <c r="H36" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1746,7 +1746,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="7"/>
       <c r="H37" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1991,6 +1991,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -2002,12 +2008,6 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H47">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2027,6 +2027,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6E01E278A50734B8A721F01C1B19487" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03d34044917dd15f7665c3faabfa0379">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="951c5514-b77c-4532-82d5-a05f2f7d58e2" xmlns:ns3="c6f516c4-2602-422c-aa9a-755893ba4f98" xmlns:ns4="3c35e321-f73a-4dae-ae38-a0459de24735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6109835e45fae7978495c991aa49747" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="951c5514-b77c-4532-82d5-a05f2f7d58e2"/>
@@ -2286,15 +2295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2307,6 +2307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{895DC2EA-9217-47D1-A436-27928D1C4E1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2322,14 +2330,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F0F638-0648-46BA-B1DF-3E4F6ADB00E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>